<commit_message>
modificaciones en visualizacion de encuesta
</commit_message>
<xml_diff>
--- a/assets/pages/Reportes/Reporte-Prueba borrador.xlsx
+++ b/assets/pages/Reportes/Reporte-Prueba borrador.xlsx
@@ -15,18 +15,66 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
+  <si>
+    <t>Nombre y Apellido Encuestador</t>
+  </si>
   <si>
     <t>Identificación del Encuestado</t>
   </si>
   <si>
-    <t>Nombre y Apellido Encuestador</t>
+    <t>Edad Encuestado</t>
   </si>
   <si>
     <t>Sexo Encuestado</t>
   </si>
   <si>
-    <t>Edad Encuestado</t>
+    <t>Alimento</t>
+  </si>
+  <si>
+    <t>NroPorcion</t>
+  </si>
+  <si>
+    <t>Frecuencia</t>
+  </si>
+  <si>
+    <t>Peso Asociado</t>
+  </si>
+  <si>
+    <t>Unidad de medida</t>
+  </si>
+  <si>
+    <t>Energia</t>
+  </si>
+  <si>
+    <t>Grasas</t>
+  </si>
+  <si>
+    <t>Hidratos de carbono</t>
+  </si>
+  <si>
+    <t>Proteínas</t>
+  </si>
+  <si>
+    <t>Donato</t>
+  </si>
+  <si>
+    <t>masculino</t>
+  </si>
+  <si>
+    <t>Mandarina</t>
+  </si>
+  <si>
+    <t>4-6 veces por semana</t>
+  </si>
+  <si>
+    <t>gr</t>
+  </si>
+  <si>
+    <t>Lechuga</t>
+  </si>
+  <si>
+    <t>Más de 1 vez al día</t>
   </si>
 </sst>
 </file>
@@ -365,7 +413,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:AW5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -373,7 +421,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:49">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -386,73 +434,628 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2">
+    <row r="2" spans="1:49">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
         <v>5</v>
       </c>
-      <c r="B2">
+      <c r="C2">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <v>0</v>
+      </c>
+      <c r="AH2">
+        <v>0</v>
+      </c>
+      <c r="AI2">
+        <v>0</v>
+      </c>
+      <c r="AJ2">
+        <v>0</v>
+      </c>
+      <c r="AK2">
+        <v>0</v>
+      </c>
+      <c r="AL2">
+        <v>0</v>
+      </c>
+      <c r="AM2">
+        <v>0</v>
+      </c>
+      <c r="AN2">
+        <v>0</v>
+      </c>
+      <c r="AO2">
+        <v>0</v>
+      </c>
+      <c r="AP2">
+        <v>0</v>
+      </c>
+      <c r="AQ2">
+        <v>0</v>
+      </c>
+      <c r="AR2">
+        <v>0</v>
+      </c>
+      <c r="AS2">
+        <v>0</v>
+      </c>
+      <c r="AT2">
+        <v>0</v>
+      </c>
+      <c r="AU2">
+        <v>0</v>
+      </c>
+      <c r="AV2">
+        <v>0</v>
+      </c>
+      <c r="AW2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:49">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3">
+        <v>154</v>
+      </c>
+      <c r="I3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3">
+        <v>135.828</v>
+      </c>
+      <c r="K3">
+        <v>69.916</v>
+      </c>
+      <c r="L3">
+        <v>151.844</v>
+      </c>
+      <c r="M3">
+        <v>16.94</v>
+      </c>
+      <c r="N3">
+        <v>0.0</v>
+      </c>
+      <c r="O3">
+        <v>0.0</v>
+      </c>
+      <c r="P3">
+        <v>0.0</v>
+      </c>
+      <c r="Q3">
+        <v>0.0</v>
+      </c>
+      <c r="R3">
+        <v>0.0</v>
+      </c>
+      <c r="S3">
+        <v>0.0</v>
+      </c>
+      <c r="T3">
+        <v>0.0</v>
+      </c>
+      <c r="U3">
+        <v>0.0</v>
+      </c>
+      <c r="V3">
+        <v>0.0</v>
+      </c>
+      <c r="W3">
+        <v>0.0</v>
+      </c>
+      <c r="X3">
+        <v>0.0</v>
+      </c>
+      <c r="Y3">
+        <v>0.0</v>
+      </c>
+      <c r="Z3">
+        <v>0.0</v>
+      </c>
+      <c r="AA3">
+        <v>0.0</v>
+      </c>
+      <c r="AB3">
+        <v>0.0</v>
+      </c>
+      <c r="AC3">
+        <v>0.0</v>
+      </c>
+      <c r="AD3">
+        <v>0.0</v>
+      </c>
+      <c r="AE3">
+        <v>0.0</v>
+      </c>
+      <c r="AF3">
+        <v>0.0</v>
+      </c>
+      <c r="AG3">
+        <v>0.0</v>
+      </c>
+      <c r="AH3">
+        <v>0.0</v>
+      </c>
+      <c r="AI3">
+        <v>0.0</v>
+      </c>
+      <c r="AJ3">
+        <v>0.0</v>
+      </c>
+      <c r="AK3">
+        <v>0.0</v>
+      </c>
+      <c r="AL3">
+        <v>0.0</v>
+      </c>
+      <c r="AM3">
+        <v>0.0</v>
+      </c>
+      <c r="AN3">
+        <v>0.0</v>
+      </c>
+      <c r="AO3">
+        <v>0.0</v>
+      </c>
+      <c r="AP3">
+        <v>0.0</v>
+      </c>
+      <c r="AQ3">
+        <v>0.0</v>
+      </c>
+      <c r="AR3">
+        <v>0.0</v>
+      </c>
+      <c r="AS3">
+        <v>0.0</v>
+      </c>
+      <c r="AT3">
+        <v>0.0</v>
+      </c>
+      <c r="AU3">
+        <v>0.0</v>
+      </c>
+      <c r="AV3">
+        <v>0.0</v>
+      </c>
+      <c r="AW3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:49">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4">
+        <v>200</v>
+      </c>
+      <c r="I4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <v>4</v>
+      </c>
+      <c r="L4">
+        <v>6</v>
+      </c>
+      <c r="M4">
+        <v>8</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>0</v>
+      </c>
+      <c r="AE4">
+        <v>0</v>
+      </c>
+      <c r="AF4">
+        <v>0</v>
+      </c>
+      <c r="AG4">
+        <v>0</v>
+      </c>
+      <c r="AH4">
+        <v>0</v>
+      </c>
+      <c r="AI4">
+        <v>0</v>
+      </c>
+      <c r="AJ4">
+        <v>0</v>
+      </c>
+      <c r="AK4">
+        <v>0</v>
+      </c>
+      <c r="AL4">
+        <v>0</v>
+      </c>
+      <c r="AM4">
+        <v>0</v>
+      </c>
+      <c r="AN4">
+        <v>0</v>
+      </c>
+      <c r="AO4">
+        <v>0</v>
+      </c>
+      <c r="AP4">
+        <v>0</v>
+      </c>
+      <c r="AQ4">
+        <v>0</v>
+      </c>
+      <c r="AR4">
+        <v>0</v>
+      </c>
+      <c r="AS4">
+        <v>0</v>
+      </c>
+      <c r="AT4">
+        <v>0</v>
+      </c>
+      <c r="AU4">
+        <v>0</v>
+      </c>
+      <c r="AV4">
+        <v>0</v>
+      </c>
+      <c r="AW4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:49">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>34</v>
-      </c>
-      <c r="D2">
-        <v>5</v>
-      </c>
-      <c r="E2">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>37</v>
-      </c>
-      <c r="D3">
-        <v>7</v>
-      </c>
-      <c r="E3">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4">
-        <v>6</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>34</v>
-      </c>
-      <c r="D4">
-        <v>5</v>
-      </c>
-      <c r="E4">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>37</v>
-      </c>
-      <c r="D5">
-        <v>7</v>
-      </c>
-      <c r="E5">
-        <v>200</v>
+      <c r="G5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5">
+        <v>0.0</v>
+      </c>
+      <c r="K5">
+        <v>0.0</v>
+      </c>
+      <c r="L5">
+        <v>0.0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <v>0</v>
+      </c>
+      <c r="AE5">
+        <v>0</v>
+      </c>
+      <c r="AF5">
+        <v>0</v>
+      </c>
+      <c r="AG5">
+        <v>0</v>
+      </c>
+      <c r="AH5">
+        <v>0</v>
+      </c>
+      <c r="AI5">
+        <v>0</v>
+      </c>
+      <c r="AJ5">
+        <v>0</v>
+      </c>
+      <c r="AK5">
+        <v>0</v>
+      </c>
+      <c r="AL5">
+        <v>0</v>
+      </c>
+      <c r="AM5">
+        <v>0</v>
+      </c>
+      <c r="AN5">
+        <v>0</v>
+      </c>
+      <c r="AO5">
+        <v>0</v>
+      </c>
+      <c r="AP5">
+        <v>0</v>
+      </c>
+      <c r="AQ5">
+        <v>0</v>
+      </c>
+      <c r="AR5">
+        <v>0</v>
+      </c>
+      <c r="AS5">
+        <v>0</v>
+      </c>
+      <c r="AT5">
+        <v>0</v>
+      </c>
+      <c r="AU5">
+        <v>0</v>
+      </c>
+      <c r="AV5">
+        <v>0</v>
+      </c>
+      <c r="AW5">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Resta dar las ultimas validaciones y arreglos en PHP y JS
</commit_message>
<xml_diff>
--- a/assets/pages/Reportes/Reporte-Prueba borrador.xlsx
+++ b/assets/pages/Reportes/Reporte-Prueba borrador.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="56">
   <si>
     <t>Nombre y Apellido Encuestador</t>
   </si>
@@ -56,7 +56,115 @@
     <t>Proteínas</t>
   </si>
   <si>
-    <t>Donato</t>
+    <t>Colesterol</t>
+  </si>
+  <si>
+    <t>Fibra Alimentaria</t>
+  </si>
+  <si>
+    <t>Sodio</t>
+  </si>
+  <si>
+    <t>Agua</t>
+  </si>
+  <si>
+    <t>Vitamina A</t>
+  </si>
+  <si>
+    <t>Vitamina B6</t>
+  </si>
+  <si>
+    <t>Vitamina B12</t>
+  </si>
+  <si>
+    <t>Vitamina C</t>
+  </si>
+  <si>
+    <t>Vitamina D</t>
+  </si>
+  <si>
+    <t>Vitamina E</t>
+  </si>
+  <si>
+    <t>Vitamina K</t>
+  </si>
+  <si>
+    <t>Almidón</t>
+  </si>
+  <si>
+    <t>Lactosa</t>
+  </si>
+  <si>
+    <t>Alcohol</t>
+  </si>
+  <si>
+    <t>Cafeína</t>
+  </si>
+  <si>
+    <t>Azúcares</t>
+  </si>
+  <si>
+    <t>Calcio</t>
+  </si>
+  <si>
+    <t>Hierro</t>
+  </si>
+  <si>
+    <t>Magnesio</t>
+  </si>
+  <si>
+    <t>Fósforo</t>
+  </si>
+  <si>
+    <t>Cinc</t>
+  </si>
+  <si>
+    <t>Cobre</t>
+  </si>
+  <si>
+    <t>Fluor</t>
+  </si>
+  <si>
+    <t>Manganeso</t>
+  </si>
+  <si>
+    <t>Selenio</t>
+  </si>
+  <si>
+    <t>Tiamina</t>
+  </si>
+  <si>
+    <t>Ácido Pantetónico</t>
+  </si>
+  <si>
+    <t>Riboflavina</t>
+  </si>
+  <si>
+    <t>Niacina</t>
+  </si>
+  <si>
+    <t>Folato</t>
+  </si>
+  <si>
+    <t>Ácido Fólico</t>
+  </si>
+  <si>
+    <t>Gasas Trans</t>
+  </si>
+  <si>
+    <t>Grasas Monoinsaturadas</t>
+  </si>
+  <si>
+    <t>Grasas Poliinsaturadas</t>
+  </si>
+  <si>
+    <t>Cloruro</t>
+  </si>
+  <si>
+    <t>Caroteno</t>
+  </si>
+  <si>
+    <t>Leandro Donato</t>
   </si>
   <si>
     <t>masculino</t>
@@ -461,10 +569,118 @@
       <c r="M1" t="s">
         <v>12</v>
       </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="2" spans="1:49">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="B2">
         <v>5</v>
@@ -473,22 +689,22 @@
         <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
       <c r="F2">
         <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -613,7 +829,7 @@
     </row>
     <row r="3" spans="1:49">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -622,34 +838,34 @@
         <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="F3">
         <v>4</v>
       </c>
       <c r="G3" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="H3">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="I3" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="J3">
-        <v>135.828</v>
+        <v>30.0</v>
       </c>
       <c r="K3">
-        <v>69.916</v>
+        <v>45.0</v>
       </c>
       <c r="L3">
-        <v>151.844</v>
+        <v>60.0</v>
       </c>
       <c r="M3">
-        <v>16.94</v>
+        <v>75.0</v>
       </c>
       <c r="N3">
         <v>0.0</v>
@@ -762,7 +978,7 @@
     </row>
     <row r="4" spans="1:49">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="B4">
         <v>6</v>
@@ -771,34 +987,34 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
       <c r="F4">
         <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="H4">
         <v>200</v>
       </c>
       <c r="I4" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="J4">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="K4">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="L4">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="M4">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="N4">
         <v>0</v>
@@ -911,7 +1127,7 @@
     </row>
     <row r="5" spans="1:49">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="B5">
         <v>6</v>
@@ -920,142 +1136,142 @@
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I5" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="J5">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="K5">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="L5">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="M5">
-        <v>0</v>
+        <v>5.0</v>
       </c>
       <c r="N5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="O5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="P5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="Q5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="R5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="S5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="T5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="U5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="V5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="W5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="X5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="Y5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="Z5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AA5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AB5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AC5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AD5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AE5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AF5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AG5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AH5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AI5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AJ5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AK5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AL5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AM5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AN5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AO5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AP5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AQ5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AR5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AS5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AT5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AU5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AV5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="AW5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>